<commit_message>
Added normal price support. Need to add photos
</commit_message>
<xml_diff>
--- a/static/assemblies.xlsx
+++ b/static/assemblies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WEB\Game-analog-searcher\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB70ABA-BF18-43CE-B16C-47670B892D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1597563-5949-42BE-9833-D31A34CDE3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9030" yWindow="3780" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5910" yWindow="3660" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assemblies" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -52,9 +52,6 @@
     <t>16GB</t>
   </si>
   <si>
-    <t>269 790 ₽</t>
-  </si>
-  <si>
     <t>GeForce RTX 3070</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>AMD Ryzen 3 3200G</t>
   </si>
   <si>
-    <t>67 900 ₽</t>
-  </si>
-  <si>
     <t>GeForce GTX 1650 Ti</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
     <t>4GB</t>
   </si>
   <si>
-    <t>25 990 ₽</t>
-  </si>
-  <si>
     <t>Ryzen 3 4300U with Radeon Graphics</t>
   </si>
   <si>
@@ -91,18 +82,12 @@
     <t>AMD Ryzen 5 3600X</t>
   </si>
   <si>
-    <t>199 500 ₽</t>
-  </si>
-  <si>
     <t>GeForce RTX 3060 Ti</t>
   </si>
   <si>
     <t>EDELWEISS PROTON</t>
   </si>
   <si>
-    <t>116 320 ₽</t>
-  </si>
-  <si>
     <t>GeForce GTX 1660 SUPER</t>
   </si>
   <si>
@@ -115,16 +100,10 @@
     <t>8GB</t>
   </si>
   <si>
-    <t>75 960 ₽</t>
-  </si>
-  <si>
     <t>GeForce GTX 1650 SUPER</t>
   </si>
   <si>
     <t>EDELWEISS CRUSADER</t>
-  </si>
-  <si>
-    <t>99 060 ₽</t>
   </si>
   <si>
     <t>https</t>
@@ -995,7 +974,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,155 +1012,155 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>269790</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2">
         <v>5142.7879999999996</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
+      <c r="D3">
+        <v>67900</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <v>1880.38</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4">
+        <v>25990</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
       </c>
       <c r="F4">
         <v>1772</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
+      <c r="D5">
+        <v>199500</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>4082.3440000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>26</v>
+      <c r="D6">
+        <v>116320</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F6">
         <v>4077.3319999999999</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>75960</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <v>3444.5630000000001</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>99060</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <v>3445.3319999999999</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>